<commit_message>
Implementation of UtitlityOutcome Feature
</commit_message>
<xml_diff>
--- a/Testdata/PRISMAPage_Data.xlsx
+++ b/Testdata/PRISMAPage_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDCB3A8-56D6-40C0-8089-26F1EBD339C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9297C89-E790-471C-9C3B-35815B578FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Interventional</t>
   </si>
@@ -70,22 +70,37 @@
     <t>totalRecordsNumber</t>
   </si>
   <si>
-    <t>\Testdata\Templates\PRISMA\Protocol - test demo123 - test demo123 - 20220801161006 - Copy (1).xlsx</t>
-  </si>
-  <si>
-    <t>\Testdata\Templates\PRISMA\Protocol - test demo123 - test demo123 - 20220801161006 - Copy (2).xlsx</t>
-  </si>
-  <si>
-    <t>\Testdata\Templates\PRISMA\sample - Copy (1).png</t>
-  </si>
-  <si>
-    <t>\Testdata\Templates\PRISMA\sample - Copy (2).png</t>
-  </si>
-  <si>
-    <t>\Testdata\Templates\PRISMA\sample - Copy (3).png</t>
-  </si>
-  <si>
-    <t>\Testdata\Templates\PRISMA\sample - Copy (4).png</t>
+    <t>Prisma_Population</t>
+  </si>
+  <si>
+    <t>ICER RRMM 2022 report</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\ICER\5. PRISMA.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\ICER\5. PRISMA_ICER.Clinical.PNG</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\ICER\5. PRISMA_ICER.QOL.PNG</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\ICER\5. PRISMA_ICER.Econ.PNG</t>
+  </si>
+  <si>
+    <t>Test_Sachin</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\Test_Sachin\13. PRISMA_AAA_mCRPC_ID Update.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\Test_Sachin\mCRPC_Clinical.PNG</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\Test_Sachin\mCRPC_Econ.PNG</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\PRISMA\Test_Sachin\mCRPC_QoL.PNG</t>
   </si>
 </sst>
 </file>
@@ -407,131 +422,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="24.44140625" style="2"/>
+    <col min="1" max="1" width="24.44140625" style="2"/>
+    <col min="2" max="2" width="67.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="24.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
-        <v>10</v>
-      </c>
       <c r="D2" s="2">
-        <v>11</v>
+        <v>500</v>
       </c>
       <c r="E2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1500</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>600</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1200</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1800</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2400</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>700</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1400</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2100</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2800</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>800</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1600</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2400</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3200</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>501</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1501</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2001</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="D8" s="2">
+        <v>601</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1201</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1801</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2401</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>701</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1401</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2101</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2801</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>801</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1601</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2401</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3201</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2">
-        <v>33</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2">
-        <v>41</v>
-      </c>
-      <c r="E5" s="2">
-        <v>42</v>
-      </c>
-      <c r="F5" s="2">
-        <v>43</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>